<commit_message>
Project Example 3 - Auto Policy Calculation is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/my/path path/test123/Example 3 - Auto Policy Calculation/AutoPolicyCalculation.xlsx
+++ b/my/path path/test123/Example 3 - Auto Policy Calculation/AutoPolicyCalculation.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OpenL\openl-demo-app-5.23.3\apache-tomcat-9.0.30\openl-demo\user-workspace\DEFAULT\Example 3 - Auto Policy Calculation\"/>
     </mc:Choice>
@@ -2627,13 +2627,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2798,15 +2798,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+  <cellStyleXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0" xfId="2">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3156,12 +3154,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="3">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -3582,15 +3578,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="15.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="50" style="1" customWidth="1"/>
-    <col min="5" max="5" width="76.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" style="1"/>
-    <col min="8" max="8" width="42.44140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="6.33203125"/>
+    <col min="2" max="2" customWidth="true" style="1" width="15.88671875"/>
+    <col min="3" max="3" customWidth="true" style="1" width="18.109375"/>
+    <col min="4" max="4" customWidth="true" style="1" width="50.0"/>
+    <col min="5" max="5" customWidth="true" style="1" width="76.88671875"/>
+    <col min="6" max="6" customWidth="true" style="1" width="18.33203125"/>
+    <col min="7" max="7" style="1" width="9.109375"/>
+    <col min="8" max="8" customWidth="true" style="1" width="42.44140625"/>
+    <col min="9" max="16384" style="1" width="9.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
@@ -4360,12 +4356,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
-    <col min="6" max="6" width="46.88671875" customWidth="1"/>
-    <col min="7" max="7" width="37" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="26.0"/>
+    <col min="4" max="4" customWidth="true" width="31.6640625"/>
+    <col min="5" max="5" customWidth="true" width="10.5546875"/>
+    <col min="6" max="6" customWidth="true" width="46.88671875"/>
+    <col min="7" max="7" customWidth="true" width="37.0"/>
+    <col min="8" max="8" customWidth="true" width="20.6640625"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
@@ -4449,9 +4445,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="14.109375" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="14.109375"/>
+    <col min="4" max="4" customWidth="true" width="23.88671875"/>
+    <col min="5" max="5" customWidth="true" width="11.44140625"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:13" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
@@ -4983,10 +4979,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="14.5546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" style="3" width="9.109375"/>
+    <col min="2" max="2" customWidth="true" style="3" width="14.5546875"/>
+    <col min="3" max="3" customWidth="true" style="3" width="34.0"/>
+    <col min="4" max="16384" style="3" width="9.109375"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21.6" thickBot="1" x14ac:dyDescent="0.45">
@@ -5715,10 +5711,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="14.33203125"/>
+    <col min="3" max="3" customWidth="true" width="17.0"/>
+    <col min="4" max="4" customWidth="true" width="15.6640625"/>
+    <col min="5" max="5" customWidth="true" width="18.33203125"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" s="1" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
@@ -5783,13 +5779,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.109375" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
-    <col min="6" max="6" width="48.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.0"/>
+    <col min="2" max="2" customWidth="true" style="13" width="16.33203125"/>
+    <col min="3" max="3" customWidth="true" width="22.6640625"/>
+    <col min="4" max="4" customWidth="true" width="23.109375"/>
+    <col min="5" max="5" customWidth="true" width="24.33203125"/>
+    <col min="6" max="6" customWidth="true" width="48.109375"/>
+    <col min="7" max="7" customWidth="true" width="16.33203125"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" ht="13.8" x14ac:dyDescent="0.3">
@@ -6219,8 +6215,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.5546875" customWidth="1"/>
-    <col min="4" max="4" width="65.6640625" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="27.5546875"/>
+    <col min="4" max="4" customWidth="true" width="65.6640625"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.8" x14ac:dyDescent="0.3">
@@ -6304,13 +6300,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.109375"/>
+    <col min="2" max="2" customWidth="true" style="13" width="11.33203125"/>
+    <col min="3" max="3" customWidth="true" width="14.88671875"/>
+    <col min="4" max="4" customWidth="true" width="31.5546875"/>
+    <col min="5" max="5" customWidth="true" width="21.6640625"/>
+    <col min="6" max="6" customWidth="true" width="25.6640625"/>
+    <col min="7" max="7" customWidth="true" width="11.6640625"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -6660,9 +6656,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="33.5546875" customWidth="1"/>
-    <col min="4" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="5" width="38.6640625" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="33.5546875"/>
+    <col min="4" max="4" customWidth="true" width="29.109375"/>
+    <col min="5" max="5" customWidth="true" width="38.6640625"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
@@ -6890,10 +6886,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="34.44140625" customWidth="1"/>
-    <col min="4" max="4" width="44.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="34.44140625"/>
+    <col min="4" max="4" customWidth="true" width="44.33203125"/>
+    <col min="5" max="5" customWidth="true" width="11.5546875"/>
+    <col min="6" max="6" customWidth="true" width="34.5546875"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" ht="13.8" x14ac:dyDescent="0.3">
@@ -6989,11 +6985,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="43" customWidth="1"/>
-    <col min="4" max="4" width="32.44140625" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="8" max="8" width="43.109375" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="43.0"/>
+    <col min="4" max="4" customWidth="true" width="32.44140625"/>
+    <col min="5" max="5" customWidth="true" width="23.44140625"/>
+    <col min="6" max="6" customWidth="true" width="10.0"/>
+    <col min="8" max="8" customWidth="true" width="43.109375"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
@@ -7102,13 +7098,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="7" customWidth="1"/>
-    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5546875" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
-    <col min="7" max="7" width="22.88671875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.5546875"/>
+    <col min="2" max="2" customWidth="true" width="7.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="4" max="4" customWidth="true" width="40.5546875"/>
+    <col min="5" max="5" customWidth="true" width="28.6640625"/>
+    <col min="6" max="6" customWidth="true" width="14.109375"/>
+    <col min="7" max="7" customWidth="true" width="22.88671875"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:6" ht="13.8" x14ac:dyDescent="0.3">
@@ -7696,13 +7692,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.44140625" customWidth="1"/>
-    <col min="17" max="17" width="24.88671875" customWidth="1"/>
-    <col min="18" max="18" width="24" customWidth="1"/>
-    <col min="19" max="19" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="16.0"/>
+    <col min="4" max="4" customWidth="true" width="18.0"/>
+    <col min="5" max="5" customWidth="true" width="21.88671875"/>
+    <col min="6" max="6" customWidth="true" width="42.44140625"/>
+    <col min="17" max="17" customWidth="true" width="24.88671875"/>
+    <col min="18" max="18" customWidth="true" width="24.0"/>
+    <col min="19" max="19" customWidth="true" width="25.33203125"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="13.8" x14ac:dyDescent="0.3">
@@ -7978,8 +7974,8 @@
       <c r="C29" s="37"/>
       <c r="D29" s="37"/>
       <c r="E29" s="37"/>
-      <c r="F29" s="84">
-        <v>150</v>
+      <c r="F29" s="84" t="n">
+        <v>1501.0</v>
       </c>
       <c r="G29" s="6"/>
     </row>

</xml_diff>